<commit_message>
This commit keeps many bugs, which I'll learn in a further
</commit_message>
<xml_diff>
--- a/private_apps/AI_fiction_or_scientific/modules/results/result_new.xlsx
+++ b/private_apps/AI_fiction_or_scientific/modules/results/result_new.xlsx
@@ -349,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,6 +374,96 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Количество предложений в тексте (ед.)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cell is empty</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Количество слов в тексте (ед.)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>777</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cell is empty</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Абсолютное количество знаков препинаний в тексте (ед.)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>136</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cell is empty</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Относительное количество знаков препинаний в тексте (%)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cell is empty</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Среднее число слов в предложении (ед.)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>32.38</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cell is empty</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Среднее число букв в слове (ед.)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cell is empty</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Create a part of the module for result generator. Fix paths bugs
</commit_message>
<xml_diff>
--- a/private_apps/AI_fiction_or_scientific/modules/results/result_new.xlsx
+++ b/private_apps/AI_fiction_or_scientific/modules/results/result_new.xlsx
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24</v>
+        <v>2147</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>777</v>
+        <v>16589</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -411,7 +411,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>136</v>
+        <v>5752</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -426,7 +426,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.5</v>
+        <v>34.67</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -441,7 +441,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>32.38</v>
+        <v>7.73</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -456,7 +456,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.8</v>
+        <v>6.29</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>

</xml_diff>